<commit_message>
fixing bug on bank account
</commit_message>
<xml_diff>
--- a/dataentry - borrower data.xlsx
+++ b/dataentry - borrower data.xlsx
@@ -322,9 +322,6 @@
     <t>FRANSISKA MAYA LESTARI</t>
   </si>
   <si>
-    <t>3471095110940000</t>
-  </si>
-  <si>
     <t>ACEH</t>
   </si>
   <si>
@@ -479,6 +476,9 @@
   </si>
   <si>
     <t>UNMARRIED</t>
+  </si>
+  <si>
+    <t>3471095110940001</t>
   </si>
 </sst>
 </file>
@@ -831,8 +831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CS2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CL1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="CU14" sqref="CU14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,7 +842,7 @@
     <col min="3" max="3" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="26.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.140625" style="1" bestFit="1" customWidth="1"/>
@@ -1246,16 +1246,16 @@
         <v>1994</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>102</v>
+        <v>154</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>101</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>103</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>104</v>
       </c>
       <c r="J2" s="1">
         <v>91</v>
@@ -1267,25 +1267,25 @@
         <v>12420</v>
       </c>
       <c r="M2" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="T2" s="1" t="s">
         <v>100</v>
@@ -1294,37 +1294,37 @@
         <v>101</v>
       </c>
       <c r="V2" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="W2" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="AD2" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="AE2" s="1" t="s">
+      <c r="AF2" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="AF2" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="AG2" s="1">
         <v>123</v>
@@ -1336,22 +1336,22 @@
         <v>10124</v>
       </c>
       <c r="AJ2" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AK2" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="AK2" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="AL2" s="1">
         <v>2132132</v>
       </c>
       <c r="AM2" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AN2" s="1">
         <v>2000</v>
       </c>
       <c r="AO2" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AP2" s="1">
         <v>12938178923</v>
@@ -1363,16 +1363,16 @@
         <v>99</v>
       </c>
       <c r="AS2" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="AT2" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="AT2" s="1" t="s">
+      <c r="AU2" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="AU2" s="1" t="s">
+      <c r="AV2" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="AV2" s="1" t="s">
-        <v>129</v>
       </c>
       <c r="AW2" s="1">
         <v>2434234</v>
@@ -1381,31 +1381,31 @@
         <v>2000</v>
       </c>
       <c r="AY2" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="AZ2" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="AZ2" s="1" t="s">
+      <c r="BA2" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="BA2" s="1" t="s">
+      <c r="BB2" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="BB2" s="1" t="s">
+      <c r="BC2" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="BD2" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="BC2" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="BD2" s="2" t="s">
+      <c r="BE2" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="BE2" s="1" t="s">
+      <c r="BF2" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="BF2" s="1" t="s">
+      <c r="BG2" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="BG2" s="1" t="s">
-        <v>137</v>
       </c>
       <c r="BH2" s="1">
         <v>231</v>
@@ -1417,10 +1417,10 @@
         <v>10124</v>
       </c>
       <c r="BK2" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="BL2" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="BM2" s="1">
         <v>123123</v>
@@ -1429,28 +1429,28 @@
         <v>23</v>
       </c>
       <c r="BO2" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="BP2" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="BP2" s="1" t="s">
+      <c r="BQ2" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="BR2" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="BQ2" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="BR2" s="1" t="s">
+      <c r="BS2" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="BS2" s="1" t="s">
+      <c r="BT2" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="BT2" s="1" t="s">
-        <v>143</v>
       </c>
       <c r="BU2" s="1">
         <v>2000</v>
       </c>
       <c r="BV2" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="BW2" s="1">
         <v>10124</v>
@@ -1462,25 +1462,25 @@
         <v>267</v>
       </c>
       <c r="BZ2" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="CA2" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="CB2" s="1">
         <v>234234</v>
       </c>
       <c r="CC2" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="CD2" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="CD2" s="1" t="s">
+      <c r="CE2" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="CF2" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="CE2" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="CF2" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="CG2" s="1">
         <v>335</v>
@@ -1489,13 +1489,13 @@
         <v>100</v>
       </c>
       <c r="CI2" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="CJ2" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="CJ2" s="1" t="s">
+      <c r="CK2" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="CK2" s="1" t="s">
-        <v>151</v>
       </c>
       <c r="CL2" s="1">
         <v>458</v>
@@ -1507,7 +1507,7 @@
         <v>10124</v>
       </c>
       <c r="CO2" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="CP2" s="1">
         <v>344534</v>
@@ -1516,10 +1516,10 @@
         <v>344</v>
       </c>
       <c r="CR2" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="CS2" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="CS2" s="2" t="s">
-        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>